<commit_message>
added the rest of the data except for two croc STLs
</commit_message>
<xml_diff>
--- a/specimens/alligator/AL_008/AL_008_joints.xlsx
+++ b/specimens/alligator/AL_008/AL_008_joints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\to_put_in_git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\muscle_maya\specimens\alligator\AL_008\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -478,12 +478,22 @@
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>

</xml_diff>